<commit_message>
'Finalização' da tabela de atividades do lab
</commit_message>
<xml_diff>
--- a/Tabela de Atividades_Guib.xlsx
+++ b/Tabela de Atividades_Guib.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ThinkTEd\Desktop\Guib\ThinTEd\projetoProex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master\Desktop\Gui\ThinTEd_2020\projetoProex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4ABA9D-A232-43F9-92B2-8B3EBFE7E127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E035FB2-7AEA-4CD5-85F2-CFF721DCEE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="18900" windowHeight="11055" xr2:uid="{30491156-B696-4076-9229-18F7AD416BE4}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="8850" xr2:uid="{30491156-B696-4076-9229-18F7AD416BE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>PLANILHA DE ATIVIDADES - GUIB</t>
   </si>
@@ -61,6 +61,36 @@
   </si>
   <si>
     <t>Realizar a pesquisa por Oficinas longas tipo Scratch</t>
+  </si>
+  <si>
+    <t>Inicio da leitura do livro gamefication 16/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio dia 16/02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizada no dia e adição das aulas de robotica 14/012 </t>
+  </si>
+  <si>
+    <t>Inicio das pesquisas e leituras dia 15/02</t>
+  </si>
+  <si>
+    <t>Alteração do GDD do game</t>
+  </si>
+  <si>
+    <t>Criação do Grafico de ritmo do game</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do Game in Unity</t>
+  </si>
+  <si>
+    <t>Data de Finalização prevista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sera realizado/craido uma versão para o dia 23/02 baseado nos testes anteriores </t>
+  </si>
+  <si>
+    <t>31/02</t>
   </si>
 </sst>
 </file>
@@ -84,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,17 +122,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -419,68 +474,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6603EA41-9D0D-43C4-84A0-16AC82EE1F54}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7">
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="7">
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7">
+        <v>43883</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="7">
+        <v>43884</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="7">
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="7">
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>